<commit_message>
Making sweeping changes (shoulda commited sooner)
</commit_message>
<xml_diff>
--- a/resources/LangMod/EN/KiriaSources.xlsx
+++ b/resources/LangMod/EN/KiriaSources.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Chara" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="226">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -529,7 +529,7 @@
     <t xml:space="preserve">Investigation Request</t>
   </si>
   <si>
-    <t xml:space="preserve">Mod_KiriaDLC.QuestKiria</t>
+    <t xml:space="preserve">QuestKiria</t>
   </si>
   <si>
     <t xml:space="preserve">kiriaDLC,main</t>
@@ -662,27 +662,6 @@
 (Try digging on the world map.)|An army of Kiria?! Defend yourself... |You've survived, maybe the stairs will unlock?|You've found a strange lab, look for clues. |The remains is clutching a capsule with something in it?</t>
   </si>
   <si>
-    <t xml:space="preserve">kiria_map_replace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lost map?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mod_KiriaDLC.QuestMapReplace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kiriaDLC,mapReplace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">地図をなくしちゃったの？新しいのを描きますよ。</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Did you lose the map? I can draw a new one.</t>
-  </si>
-  <si>
     <t xml:space="preserve">unknown_JP</t>
   </si>
   <si>
@@ -809,57 +788,6 @@
     <t xml:space="preserve">A hand drawn map provided by Kiria</t>
   </si>
   <si>
-    <t xml:space="preserve">kiriaTool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">キリアアイテムツール</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kiria Item Tool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_tool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rock/1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">granite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KiriaItemTool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">noWish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">遺伝子</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nanomachine Gene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KiriaGene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gacha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">生物の遺伝的情報が刻まれている。</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It bears the genetic traits of the organism.</t>
-  </si>
-  <si>
     <t xml:space="preserve">corpse_ryozu</t>
   </si>
   <si>
@@ -869,7 +797,7 @@
     <t xml:space="preserve">653,652,656,657,658,659,-659</t>
   </si>
   <si>
-    <t xml:space="preserve">KiriaCorpse</t>
+    <t xml:space="preserve">RyozuCorpse</t>
   </si>
   <si>
     <t xml:space="preserve">parent</t>
@@ -932,7 +860,7 @@
     <t xml:space="preserve">Strange factory</t>
   </si>
   <si>
-    <t xml:space="preserve">Mod_KiriaDLC.Zone_KiriaDungeon</t>
+    <t xml:space="preserve">Zone_KiriaDungeon</t>
   </si>
   <si>
     <t xml:space="preserve">DungeonFactory</t>
@@ -1226,10 +1154,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1240,6 +1164,10 @@
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1444,10 +1372,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J6" activeCellId="1" sqref="A4 J6"/>
+      <selection pane="bottomLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2152,10 +2080,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B5" activeCellId="1" sqref="A4 B5"/>
+      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -2323,10 +2251,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N22" activeCellId="1" sqref="A4 N22"/>
+      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2345,13 +2273,13 @@
   </sheetPr>
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="14.29"/>
@@ -2672,22 +2600,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="M4" activeCellId="1" sqref="A4 M4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="16.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="9.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="19.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="28.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="18.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="10" width="234.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="10" width="136.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="21" width="208"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="10" width="14.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="10" width="11.73"/>
@@ -2748,7 +2676,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>140</v>
       </c>
@@ -2771,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="5" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>145</v>
@@ -2783,38 +2711,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="I5" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="M5" s="21" t="s">
-        <v>153</v>
-      </c>
-    </row>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2831,22 +2735,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BT7"/>
+  <dimension ref="A1:BT1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N8" activeCellId="1" sqref="A4 N8"/>
+      <selection pane="bottomRight" activeCell="AH6" activeCellId="0" sqref="AH6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="11.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="25.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="10" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="10" width="27.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2857,22 +2761,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>32</v>
@@ -2893,13 +2797,13 @@
         <v>10</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>8</v>
@@ -2920,15 +2824,15 @@
         <v>13</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="AA1" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA1" s="22" t="s">
         <v>111</v>
       </c>
       <c r="AB1" s="2" t="s">
@@ -2941,13 +2845,13 @@
         <v>17</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="AF1" s="23" t="s">
-        <v>165</v>
+        <v>157</v>
+      </c>
+      <c r="AF1" s="22" t="s">
+        <v>158</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="AH1" s="2" t="s">
         <v>21</v>
@@ -2956,19 +2860,19 @@
         <v>29</v>
       </c>
       <c r="AJ1" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="AO1" s="2" t="s">
         <v>37</v>
@@ -2977,28 +2881,28 @@
         <v>38</v>
       </c>
       <c r="AQ1" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="AR1" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="AS1" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="AT1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="AW1" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="AX1" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>46</v>
@@ -3104,7 +3008,7 @@
       <c r="Z2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" s="23" t="s">
+      <c r="AA2" s="22" t="s">
         <v>49</v>
       </c>
       <c r="AB2" s="2" t="s">
@@ -3119,7 +3023,7 @@
       <c r="AE2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AF2" s="23" t="s">
+      <c r="AF2" s="22" t="s">
         <v>49</v>
       </c>
       <c r="AG2" s="2" t="s">
@@ -3208,14 +3112,14 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="3" t="s">
@@ -3241,23 +3145,23 @@
       </c>
       <c r="X3" s="2"/>
       <c r="Y3" s="3" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="Z3" s="2"/>
-      <c r="AA3" s="24" t="n">
+      <c r="AA3" s="23" t="n">
         <v>100</v>
       </c>
-      <c r="AB3" s="25" t="n">
+      <c r="AB3" s="24" t="n">
         <v>1</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="AD3" s="2"/>
       <c r="AE3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AF3" s="24" t="n">
+      <c r="AF3" s="23" t="n">
         <v>1000</v>
       </c>
       <c r="AG3" s="2"/>
@@ -3305,31 +3209,31 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="K4" s="5" t="n">
         <v>100</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="N4" s="5" t="n">
         <v>1713</v>
@@ -3338,10 +3242,10 @@
         <v>100</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="AA4" s="5" t="n">
         <v>3500</v>
@@ -3365,222 +3269,88 @@
         <v>0</v>
       </c>
       <c r="AH4" s="5" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="AJ4" s="5" t="n">
         <v>1</v>
       </c>
       <c r="AT4" s="5" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="AY4" s="6" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="AZ4" s="5" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>196</v>
+      <c r="A5" s="10" t="s">
+        <v>189</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>178</v>
+        <v>124</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>171</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="K5" s="5" t="n">
+        <v>125</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="K5" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="N5" s="5" t="n">
-        <v>1810</v>
-      </c>
-      <c r="S5" s="5" t="n">
+      <c r="N5" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="S5" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="W5" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="Y5" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="AA5" s="5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="AB5" s="5" t="n">
+      <c r="W5" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y5" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA5" s="10" t="n">
+        <v>2686</v>
+      </c>
+      <c r="AB5" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="AC5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="5" t="n">
+      <c r="AC5" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="AF5" s="5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="AG5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="AJ5" s="5" t="n">
+      <c r="AF5" s="10" t="n">
+        <v>4000</v>
+      </c>
+      <c r="AG5" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="AJ5" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="AT5" s="5" t="s">
-        <v>203</v>
+      <c r="AT5" s="10" t="s">
+        <v>186</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="K6" s="5" t="n">
-        <v>100</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="N6" s="5" t="n">
-        <v>549</v>
-      </c>
-      <c r="S6" s="5" t="n">
-        <v>100</v>
-      </c>
-      <c r="W6" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="Y6" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AA6" s="5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="AB6" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="5" t="n">
-        <v>100</v>
-      </c>
-      <c r="AF6" s="5" t="n">
-        <v>200</v>
-      </c>
-      <c r="AG6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="AJ6" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV6" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="AY6" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="AZ6" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="K7" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="S7" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="W7" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y7" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA7" s="10" t="n">
-        <v>2686</v>
-      </c>
-      <c r="AB7" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="AF7" s="10" t="n">
-        <v>4000</v>
-      </c>
-      <c r="AG7" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="AJ7" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT7" s="10" t="s">
-        <v>193</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3602,13 +3372,15 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I10" activeCellId="1" sqref="A4 I10"/>
+      <selection pane="bottomLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3616,7 +3388,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="C1" s="26" t="s">
         <v>2</v>
@@ -3634,49 +3406,49 @@
         <v>16</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="I1" s="26" t="s">
         <v>111</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="L1" s="26" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="M1" s="26" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="N1" s="26" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="O1" s="26" t="s">
         <v>20</v>
       </c>
       <c r="P1" s="26" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="Q1" s="26" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="R1" s="26" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="S1" s="26" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="T1" s="26" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="U1" s="26" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="V1" s="26" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="W1" s="26" t="s">
         <v>46</v>
@@ -3771,7 +3543,7 @@
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
       <c r="E3" s="26" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="F3" s="26" t="n">
         <v>1</v>
@@ -3794,7 +3566,7 @@
         <v>0</v>
       </c>
       <c r="R3" s="26" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="S3" s="27"/>
       <c r="T3" s="27"/>
@@ -3808,22 +3580,22 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>0</v>
@@ -3832,16 +3604,16 @@
         <v>0</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="P4" s="5" t="n">
         <v>0</v>
@@ -3850,30 +3622,30 @@
         <v>0</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="F5" s="5" t="n">
         <v>1</v>
@@ -3885,7 +3657,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>63</v>
@@ -3897,13 +3669,13 @@
         <v>0</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="U5" s="6" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>